<commit_message>
Ajout de l'injection des formats d'enseignement et des structures porteuses
</commit_message>
<xml_diff>
--- a/maquette-type.xlsx
+++ b/maquette-type.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\apereir\Desktop\En cours\En cours Maquettes\scripts\maquettes-xl2json\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60063C83-C132-4EE5-99EC-7A1BA257FBFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5D81A9C-C61F-422D-B590-140075185B8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{A6F31FBE-6D40-488E-B868-E7547D61F047}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A6F31FBE-6D40-488E-B868-E7547D61F047}"/>
   </bookViews>
   <sheets>
     <sheet name="Format complet sans décorations" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="191">
   <si>
     <t>EC</t>
   </si>
@@ -586,6 +586,36 @@
   </si>
   <si>
     <t>MED020</t>
+  </si>
+  <si>
+    <t>Structures porteuses</t>
+  </si>
+  <si>
+    <t>Formats - modalités</t>
+  </si>
+  <si>
+    <t>Formats - volume horaire</t>
+  </si>
+  <si>
+    <t>Selon référentiel (codes séparés par virgule)</t>
+  </si>
+  <si>
+    <t>Nombre entier (0 par défaut)</t>
+  </si>
+  <si>
+    <t>Format 12h30 ou 12:30</t>
+  </si>
+  <si>
+    <t>Formats - type heures</t>
+  </si>
+  <si>
+    <t>Formats - nombre groupes</t>
+  </si>
+  <si>
+    <t>Formats - seuil dédoublement</t>
+  </si>
+  <si>
+    <t>Selon référentiel (obligatoire si les modalités sont indiquées)</t>
   </si>
 </sst>
 </file>
@@ -593,9 +623,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="171" formatCode="[$-40C]General"/>
-    <numFmt numFmtId="172" formatCode="&quot; &quot;#,##0.00&quot;   &quot;;&quot;-&quot;#,##0.00&quot;   &quot;;&quot; -&quot;00&quot;   &quot;;@&quot; &quot;"/>
-    <numFmt numFmtId="173" formatCode="#,##0.00&quot; &quot;[$€-40C];[Red]&quot;-&quot;#,##0.00&quot; &quot;[$€-40C]"/>
+    <numFmt numFmtId="164" formatCode="[$-40C]General"/>
+    <numFmt numFmtId="165" formatCode="&quot; &quot;#,##0.00&quot;   &quot;;&quot;-&quot;#,##0.00&quot;   &quot;;&quot; -&quot;00&quot;   &quot;;@&quot; &quot;"/>
+    <numFmt numFmtId="166" formatCode="#,##0.00&quot; &quot;[$€-40C];[Red]&quot;-&quot;#,##0.00&quot; &quot;[$€-40C]"/>
   </numFmts>
   <fonts count="29">
     <font>
@@ -958,8 +988,8 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
-    <xf numFmtId="172" fontId="16" fillId="0" borderId="0"/>
-    <xf numFmtId="171" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0">
       <alignment horizontal="center"/>
     </xf>
@@ -967,28 +997,28 @@
       <alignment horizontal="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="173" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="19" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="23" fillId="0" borderId="0"/>
-    <xf numFmtId="171" fontId="22" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
-    <xf numFmtId="171" fontId="23" fillId="0" borderId="0"/>
-    <xf numFmtId="171" fontId="23" fillId="0" borderId="0"/>
-    <xf numFmtId="171" fontId="25" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
-    <xf numFmtId="173" fontId="26" fillId="0" borderId="0"/>
+    <xf numFmtId="166" fontId="26" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1098,6 +1128,12 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="22" fontId="9" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="29">
     <cellStyle name="Excel Built-in Normal" xfId="3" xr:uid="{B5E05A5B-D7AC-4D1C-928B-A110500C8CDE}"/>
@@ -1130,7 +1166,761 @@
     <cellStyle name="Result2 2" xfId="25" xr:uid="{C89B0715-43C1-48F0-9C01-C019D6CCF141}"/>
     <cellStyle name="Texte explicatif 2" xfId="15" xr:uid="{F8296A05-B0FD-4A9C-A976-1DD3C341052F}"/>
   </cellStyles>
-  <dxfs count="54">
+  <dxfs count="46">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1165,856 +1955,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </left>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2029,48 +1969,54 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0F039B8D-4F73-4F71-816E-79D8DD07FF1D}" name="Tableau1" displayName="Tableau1" ref="A1:AM3" totalsRowShown="0" headerRowDxfId="53" dataDxfId="51" headerRowBorderDxfId="52" tableBorderDxfId="50" totalsRowBorderDxfId="49">
-  <autoFilter ref="A1:AM3" xr:uid="{0F039B8D-4F73-4F71-816E-79D8DD07FF1D}"/>
-  <tableColumns count="39">
-    <tableColumn id="1" xr3:uid="{BA1FF67E-A285-4DC9-A88A-D3161AF85CDF}" name="Type objet" dataDxfId="48"/>
-    <tableColumn id="3" xr3:uid="{7504398C-07C2-4F18-9E4F-B24B0EEFC607}" name="Nature objet" dataDxfId="47"/>
-    <tableColumn id="2" xr3:uid="{9465B86C-1C8A-47C9-8DE0-27C5143473B9}" name="Code objet" dataDxfId="46"/>
-    <tableColumn id="6" xr3:uid="{01197EF2-8F7E-416D-87BE-211104178B19}" name="Libellé" dataDxfId="45"/>
-    <tableColumn id="8" xr3:uid="{178F97CB-CD98-4DF4-9B3B-88D67784A1AA}" name="Libellé long" dataDxfId="14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0F039B8D-4F73-4F71-816E-79D8DD07FF1D}" name="Tableau1" displayName="Tableau1" ref="A1:AS3" totalsRowShown="0" headerRowDxfId="42" dataDxfId="40" headerRowBorderDxfId="41" tableBorderDxfId="39" totalsRowBorderDxfId="38">
+  <autoFilter ref="A1:AS3" xr:uid="{0F039B8D-4F73-4F71-816E-79D8DD07FF1D}"/>
+  <tableColumns count="45">
+    <tableColumn id="1" xr3:uid="{BA1FF67E-A285-4DC9-A88A-D3161AF85CDF}" name="Type objet" dataDxfId="37"/>
+    <tableColumn id="3" xr3:uid="{7504398C-07C2-4F18-9E4F-B24B0EEFC607}" name="Nature objet" dataDxfId="36"/>
+    <tableColumn id="2" xr3:uid="{9465B86C-1C8A-47C9-8DE0-27C5143473B9}" name="Code objet" dataDxfId="35"/>
+    <tableColumn id="6" xr3:uid="{01197EF2-8F7E-416D-87BE-211104178B19}" name="Libellé" dataDxfId="34"/>
+    <tableColumn id="8" xr3:uid="{178F97CB-CD98-4DF4-9B3B-88D67784A1AA}" name="Libellé long" dataDxfId="33"/>
     <tableColumn id="13" xr3:uid="{E5AC1167-2E73-40D7-8183-D7484EA2F3AE}" name="PIA"/>
-    <tableColumn id="9" xr3:uid="{F8670986-ECED-46AC-BE3A-65280B926387}" name="ECTS objet" dataDxfId="16"/>
-    <tableColumn id="10" xr3:uid="{492B8453-2431-4BA1-9E89-D32C0957EDE0}" name="Code parent" dataDxfId="15"/>
-    <tableColumn id="20" xr3:uid="{26C11A25-FC98-4B71-B8A2-25788CD2B149}" name="Mutualisé" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{6813EE45-5417-475E-AC92-8D2734747C05}" name="Plage MIN" dataDxfId="44"/>
-    <tableColumn id="5" xr3:uid="{387629FB-EF79-4A94-AF68-1297523114CB}" name="Plage MAX" dataDxfId="43"/>
-    <tableColumn id="7" xr3:uid="{6487F377-EED9-48BA-A0F8-4A81D873DD01}" name="Distanciel" dataDxfId="42"/>
-    <tableColumn id="11" xr3:uid="{73D73693-FBE4-447E-87A3-B8013A93014D}" name="Stage" dataDxfId="41"/>
-    <tableColumn id="12" xr3:uid="{079EC281-2E43-49C5-BB70-8E623D48D2BB}" name="Capacité accueil" dataDxfId="40"/>
-    <tableColumn id="14" xr3:uid="{81B85A8A-5130-4E33-BEC7-14C40B480F8E}" name="Structure principale" dataDxfId="39"/>
-    <tableColumn id="19" xr3:uid="{1D4BC2ED-329F-4239-B9B3-B6178725F3C4}" name="Type formation" dataDxfId="38"/>
-    <tableColumn id="21" xr3:uid="{843B1EE6-D73E-42E2-9F41-34613C9BD26B}" name="Syllabus - objectifs" dataDxfId="37"/>
-    <tableColumn id="22" xr3:uid="{439B1D33-D1DA-42A4-97DD-0E7753B45ED7}" name="Syllabus - description" dataDxfId="36"/>
-    <tableColumn id="23" xr3:uid="{7CAE92B6-CB33-4DC4-979D-CFF975E75B01}" name="Syllabus - ouverture mobilité entrante" dataDxfId="35"/>
-    <tableColumn id="24" xr3:uid="{9503C41F-78D9-4DD7-BA1C-4A72C20CECBB}" name="Syllabus - langue enseignement" dataDxfId="34"/>
-    <tableColumn id="25" xr3:uid="{0F114DF4-A772-4246-BFA4-E5EADBF9FBC8}" name="Syllabus - prérequis" dataDxfId="33"/>
-    <tableColumn id="26" xr3:uid="{24945D32-A70D-4E65-900D-E45A82AB5A05}" name="Syllabus - bibliographie" dataDxfId="32"/>
-    <tableColumn id="27" xr3:uid="{C613C925-D074-4B70-BC6C-D7579D55942E}" name="Syllabus - contacts" dataDxfId="31"/>
-    <tableColumn id="28" xr3:uid="{F4FBD0B9-F6B1-4A70-9C69-08FE8BB374DA}" name="Syllabus - autres informations" dataDxfId="30"/>
-    <tableColumn id="29" xr3:uid="{25076670-8FBF-4B5A-BC03-AAB90E12326B}" name="Syllabus - modalités enseignement" dataDxfId="29"/>
-    <tableColumn id="30" xr3:uid="{B9BBA5EA-92C4-43C5-8B4E-9E9648E7B13E}" name="Syllabus - volume horaire" dataDxfId="28"/>
-    <tableColumn id="31" xr3:uid="{AAAE5565-606B-4E1C-9FD8-99E9CD898B38}" name="Syllabus - coefficient" dataDxfId="27"/>
-    <tableColumn id="32" xr3:uid="{5498CC05-730A-4838-ADF5-C8C1D9E79021}" name="Syllabus - modalités évaluation" dataDxfId="26"/>
-    <tableColumn id="33" xr3:uid="{926DEFC4-5CBB-45C6-9258-AB7C8F37849C}" name="SISE - type diplôme" dataDxfId="25"/>
+    <tableColumn id="9" xr3:uid="{F8670986-ECED-46AC-BE3A-65280B926387}" name="ECTS objet" dataDxfId="32"/>
+    <tableColumn id="10" xr3:uid="{492B8453-2431-4BA1-9E89-D32C0957EDE0}" name="Code parent" dataDxfId="31"/>
+    <tableColumn id="20" xr3:uid="{26C11A25-FC98-4B71-B8A2-25788CD2B149}" name="Mutualisé" dataDxfId="30"/>
+    <tableColumn id="4" xr3:uid="{6813EE45-5417-475E-AC92-8D2734747C05}" name="Plage MIN" dataDxfId="29"/>
+    <tableColumn id="5" xr3:uid="{387629FB-EF79-4A94-AF68-1297523114CB}" name="Plage MAX" dataDxfId="28"/>
+    <tableColumn id="7" xr3:uid="{6487F377-EED9-48BA-A0F8-4A81D873DD01}" name="Distanciel" dataDxfId="27"/>
+    <tableColumn id="11" xr3:uid="{73D73693-FBE4-447E-87A3-B8013A93014D}" name="Stage" dataDxfId="26"/>
+    <tableColumn id="12" xr3:uid="{079EC281-2E43-49C5-BB70-8E623D48D2BB}" name="Capacité accueil" dataDxfId="25"/>
+    <tableColumn id="14" xr3:uid="{81B85A8A-5130-4E33-BEC7-14C40B480F8E}" name="Structure principale" dataDxfId="24"/>
+    <tableColumn id="19" xr3:uid="{1D4BC2ED-329F-4239-B9B3-B6178725F3C4}" name="Type formation" dataDxfId="23"/>
+    <tableColumn id="15" xr3:uid="{C2B2490D-815D-40D6-9C11-63539FA4C1E7}" name="Structures porteuses"/>
+    <tableColumn id="16" xr3:uid="{711E9C20-D895-45E9-A114-2E14A75AE220}" name="Formats - modalités"/>
+    <tableColumn id="17" xr3:uid="{B0B68448-C1C4-4A12-99E8-817441FE3C16}" name="Formats - type heures"/>
+    <tableColumn id="18" xr3:uid="{47C56DB4-7A85-4F6B-B14E-0272B97C5BEB}" name="Formats - volume horaire"/>
+    <tableColumn id="44" xr3:uid="{0D4BBC6F-9FC2-4C24-B9A9-83D9B3E44FF0}" name="Formats - nombre groupes"/>
+    <tableColumn id="45" xr3:uid="{DD3743CA-AAA9-4694-BDB8-04B2A988F9CA}" name="Formats - seuil dédoublement"/>
+    <tableColumn id="21" xr3:uid="{843B1EE6-D73E-42E2-9F41-34613C9BD26B}" name="Syllabus - objectifs" dataDxfId="22"/>
+    <tableColumn id="22" xr3:uid="{439B1D33-D1DA-42A4-97DD-0E7753B45ED7}" name="Syllabus - description" dataDxfId="21"/>
+    <tableColumn id="23" xr3:uid="{7CAE92B6-CB33-4DC4-979D-CFF975E75B01}" name="Syllabus - ouverture mobilité entrante" dataDxfId="20"/>
+    <tableColumn id="24" xr3:uid="{9503C41F-78D9-4DD7-BA1C-4A72C20CECBB}" name="Syllabus - langue enseignement" dataDxfId="19"/>
+    <tableColumn id="25" xr3:uid="{0F114DF4-A772-4246-BFA4-E5EADBF9FBC8}" name="Syllabus - prérequis" dataDxfId="18"/>
+    <tableColumn id="26" xr3:uid="{24945D32-A70D-4E65-900D-E45A82AB5A05}" name="Syllabus - bibliographie" dataDxfId="17"/>
+    <tableColumn id="27" xr3:uid="{C613C925-D074-4B70-BC6C-D7579D55942E}" name="Syllabus - contacts" dataDxfId="16"/>
+    <tableColumn id="28" xr3:uid="{F4FBD0B9-F6B1-4A70-9C69-08FE8BB374DA}" name="Syllabus - autres informations" dataDxfId="15"/>
+    <tableColumn id="29" xr3:uid="{25076670-8FBF-4B5A-BC03-AAB90E12326B}" name="Syllabus - modalités enseignement" dataDxfId="14"/>
+    <tableColumn id="30" xr3:uid="{B9BBA5EA-92C4-43C5-8B4E-9E9648E7B13E}" name="Syllabus - volume horaire" dataDxfId="13"/>
+    <tableColumn id="31" xr3:uid="{AAAE5565-606B-4E1C-9FD8-99E9CD898B38}" name="Syllabus - coefficient" dataDxfId="12"/>
+    <tableColumn id="32" xr3:uid="{5498CC05-730A-4838-ADF5-C8C1D9E79021}" name="Syllabus - modalités évaluation" dataDxfId="11"/>
+    <tableColumn id="33" xr3:uid="{926DEFC4-5CBB-45C6-9258-AB7C8F37849C}" name="SISE - type diplôme" dataDxfId="10"/>
     <tableColumn id="34" xr3:uid="{EA4EA027-ED14-4DA3-A532-58D76A59190E}" name="SISE - code diplôme" dataDxfId="9"/>
-    <tableColumn id="35" xr3:uid="{1868BDEE-EAEC-4246-AA88-B45FC2F23CAB}" name="SISE - niveau diplôme SISE" dataDxfId="7"/>
-    <tableColumn id="36" xr3:uid="{44AEC1EA-EF1D-47CB-B98E-0964862967FF}" name="SISE - parcours-type" dataDxfId="8"/>
-    <tableColumn id="37" xr3:uid="{0BC82DF8-EF3F-46C6-9CE3-BF2F682E7EED}" name="SISE - domaine formation" dataDxfId="24"/>
-    <tableColumn id="38" xr3:uid="{257739AB-3A09-46A6-9600-44BC34413430}" name="SISE - mention" dataDxfId="23"/>
-    <tableColumn id="39" xr3:uid="{15F9D87A-1B9D-4A42-983C-5A9FE99D0322}" name="SISE - champ formation" dataDxfId="22"/>
-    <tableColumn id="40" xr3:uid="{D3C47171-A1B9-4104-88B8-596268A0FDEF}" name="SISE - niveau diplôme" dataDxfId="21"/>
-    <tableColumn id="41" xr3:uid="{C72D07E6-20C8-476F-9FD4-8D9791FB1C06}" name="SISE - déclinaison" dataDxfId="20"/>
-    <tableColumn id="42" xr3:uid="{94F15C63-346A-4FAE-B411-4BA84BEA21E7}" name="Aglae - habilité bourses" dataDxfId="19"/>
-    <tableColumn id="43" xr3:uid="{0E47B228-4380-4D0A-A175-FBF1292E0FC1}" name="Aglae - niveau" dataDxfId="18"/>
+    <tableColumn id="35" xr3:uid="{1868BDEE-EAEC-4246-AA88-B45FC2F23CAB}" name="SISE - niveau diplôme SISE" dataDxfId="8"/>
+    <tableColumn id="36" xr3:uid="{44AEC1EA-EF1D-47CB-B98E-0964862967FF}" name="SISE - parcours-type" dataDxfId="7"/>
+    <tableColumn id="37" xr3:uid="{0BC82DF8-EF3F-46C6-9CE3-BF2F682E7EED}" name="SISE - domaine formation" dataDxfId="6"/>
+    <tableColumn id="38" xr3:uid="{257739AB-3A09-46A6-9600-44BC34413430}" name="SISE - mention" dataDxfId="5"/>
+    <tableColumn id="39" xr3:uid="{15F9D87A-1B9D-4A42-983C-5A9FE99D0322}" name="SISE - champ formation" dataDxfId="4"/>
+    <tableColumn id="40" xr3:uid="{D3C47171-A1B9-4104-88B8-596268A0FDEF}" name="SISE - niveau diplôme" dataDxfId="3"/>
+    <tableColumn id="41" xr3:uid="{C72D07E6-20C8-476F-9FD4-8D9791FB1C06}" name="SISE - déclinaison" dataDxfId="2"/>
+    <tableColumn id="42" xr3:uid="{94F15C63-346A-4FAE-B411-4BA84BEA21E7}" name="Aglae - habilité bourses" dataDxfId="1"/>
+    <tableColumn id="43" xr3:uid="{0E47B228-4380-4D0A-A175-FBF1292E0FC1}" name="Aglae - niveau" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2373,20 +2319,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{344DF7D5-D639-4355-89FB-833EF1843A63}">
-  <dimension ref="A1:AM47"/>
+  <dimension ref="A1:AS47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AF5" sqref="AF5"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16.2" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="16.88671875" customWidth="1"/>
-    <col min="2" max="2" width="11.21875" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" customWidth="1"/>
     <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="55.33203125" customWidth="1"/>
     <col min="5" max="5" width="55.33203125" style="7" customWidth="1"/>
-    <col min="6" max="6" width="19.21875" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" customWidth="1"/>
     <col min="7" max="7" width="14.44140625" style="8" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="24.6640625" style="15" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20" customWidth="1"/>
@@ -2394,16 +2338,22 @@
     <col min="11" max="11" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="15" width="14.6640625" style="7" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="19.5546875" style="7" customWidth="1"/>
-    <col min="17" max="19" width="14.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="22.33203125" style="7" customWidth="1"/>
-    <col min="21" max="21" width="20.44140625" style="7" customWidth="1"/>
-    <col min="22" max="24" width="14.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="19.44140625" style="7" customWidth="1"/>
-    <col min="26" max="39" width="14.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="16.33203125" customWidth="1"/>
+    <col min="17" max="17" width="17.109375" style="7" customWidth="1"/>
+    <col min="18" max="18" width="19.5546875" style="7" customWidth="1"/>
+    <col min="19" max="19" width="17.44140625" style="7" customWidth="1"/>
+    <col min="20" max="20" width="19.5546875" style="7" customWidth="1"/>
+    <col min="21" max="22" width="17" style="7" customWidth="1"/>
+    <col min="23" max="24" width="14.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="18.109375" style="7" customWidth="1"/>
+    <col min="26" max="26" width="22.33203125" style="7" customWidth="1"/>
+    <col min="27" max="27" width="20.44140625" style="7" customWidth="1"/>
+    <col min="28" max="30" width="14.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="19.44140625" style="7" customWidth="1"/>
+    <col min="32" max="45" width="14.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" s="2" customFormat="1" ht="55.8" customHeight="1">
+    <row r="1" spans="1:45" s="2" customFormat="1" ht="55.95" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -2453,76 +2403,94 @@
         <v>15</v>
       </c>
       <c r="Q1" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="W1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:39" s="2" customFormat="1" ht="61.8" customHeight="1">
+    <row r="2" spans="1:45" s="2" customFormat="1" ht="61.95" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>23</v>
       </c>
@@ -2572,22 +2540,22 @@
         <v>27</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>52</v>
+        <v>184</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>28</v>
+        <v>190</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>52</v>
+        <v>186</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>52</v>
+        <v>185</v>
       </c>
       <c r="W2" s="3" t="s">
         <v>52</v>
@@ -2596,34 +2564,34 @@
         <v>52</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="Z2" s="3" t="s">
         <v>52</v>
       </c>
       <c r="AA2" s="3" t="s">
-        <v>18</v>
+        <v>52</v>
       </c>
       <c r="AB2" s="3" t="s">
         <v>52</v>
       </c>
       <c r="AC2" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AD2" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AE2" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AF2" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AG2" s="3" t="s">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="AH2" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AI2" s="3" t="s">
         <v>53</v>
@@ -2635,13 +2603,31 @@
         <v>53</v>
       </c>
       <c r="AL2" s="3" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="AM2" s="3" t="s">
         <v>53</v>
       </c>
+      <c r="AN2" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="AO2" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="AP2" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="AQ2" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="AR2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="AS2" s="3" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="3" spans="1:39" s="2" customFormat="1" ht="16.2" customHeight="1">
+    <row r="3" spans="1:45" s="2" customFormat="1" ht="16.2" customHeight="1">
       <c r="A3" s="33"/>
       <c r="B3" s="33"/>
       <c r="C3" s="33"/>
@@ -2681,8 +2667,14 @@
       <c r="AK3" s="33"/>
       <c r="AL3" s="33"/>
       <c r="AM3" s="33"/>
+      <c r="AN3" s="33"/>
+      <c r="AO3" s="33"/>
+      <c r="AP3" s="33"/>
+      <c r="AQ3" s="33"/>
+      <c r="AR3" s="33"/>
+      <c r="AS3" s="33"/>
     </row>
-    <row r="4" spans="1:39" s="16" customFormat="1" ht="57.6" customHeight="1">
+    <row r="4" spans="1:45" s="16" customFormat="1" ht="57.6" customHeight="1">
       <c r="A4" s="37" t="s">
         <v>70</v>
       </c>
@@ -2715,78 +2707,84 @@
       <c r="P4" s="36">
         <v>0</v>
       </c>
-      <c r="Q4" s="37" t="s">
+      <c r="Q4" s="36"/>
+      <c r="R4" s="36"/>
+      <c r="S4" s="36"/>
+      <c r="T4" s="36"/>
+      <c r="U4" s="36"/>
+      <c r="V4" s="36"/>
+      <c r="W4" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="R4" s="37" t="s">
+      <c r="X4" s="37" t="s">
         <v>178</v>
       </c>
-      <c r="S4" s="37" t="b">
+      <c r="Y4" s="37" t="b">
         <v>1</v>
       </c>
-      <c r="T4" s="37" t="s">
+      <c r="Z4" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="U4" s="37" t="s">
+      <c r="AA4" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="V4" s="37" t="s">
+      <c r="AB4" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="W4" s="37" t="s">
+      <c r="AC4" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="X4" s="37" t="s">
+      <c r="AD4" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="Y4" s="37" t="s">
+      <c r="AE4" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="Z4" s="37" t="s">
+      <c r="AF4" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="AA4" s="36">
+      <c r="AG4" s="36">
         <v>4</v>
       </c>
-      <c r="AB4" s="37" t="s">
+      <c r="AH4" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="AC4" s="37" t="s">
+      <c r="AI4" s="37" t="s">
         <v>179</v>
       </c>
-      <c r="AD4" s="36">
+      <c r="AJ4" s="36">
         <v>1000218</v>
       </c>
-      <c r="AE4" s="36">
+      <c r="AK4" s="36">
         <v>2</v>
       </c>
-      <c r="AF4" s="36" t="s">
+      <c r="AL4" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="AG4" s="36" t="s">
+      <c r="AM4" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="AH4" s="36" t="s">
+      <c r="AN4" s="36" t="s">
         <v>180</v>
       </c>
-      <c r="AI4" s="36" t="s">
+      <c r="AO4" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="AJ4" s="36" t="s">
+      <c r="AP4" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="AK4" s="37" t="s">
+      <c r="AQ4" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="AL4" s="36" t="b">
+      <c r="AR4" s="36" t="b">
         <v>1</v>
       </c>
-      <c r="AM4" s="36" t="str">
+      <c r="AS4" s="36" t="str">
         <f>"02"</f>
         <v>02</v>
       </c>
     </row>
-    <row r="5" spans="1:39" ht="16.2" customHeight="1">
+    <row r="5" spans="1:45" ht="16.2" customHeight="1">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -2795,7 +2793,7 @@
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
     </row>
-    <row r="6" spans="1:39" ht="22.8" customHeight="1">
+    <row r="6" spans="1:45" ht="22.95" customHeight="1">
       <c r="A6" s="9" t="s">
         <v>73</v>
       </c>
@@ -2851,8 +2849,14 @@
       <c r="AK6" s="10"/>
       <c r="AL6" s="10"/>
       <c r="AM6" s="10"/>
+      <c r="AN6" s="10"/>
+      <c r="AO6" s="10"/>
+      <c r="AP6" s="10"/>
+      <c r="AQ6" s="10"/>
+      <c r="AR6" s="10"/>
+      <c r="AS6" s="10"/>
     </row>
-    <row r="7" spans="1:39" ht="24" customHeight="1">
+    <row r="7" spans="1:45" ht="24" customHeight="1">
       <c r="A7" s="11" t="s">
         <v>77</v>
       </c>
@@ -2906,8 +2910,14 @@
       <c r="AK7" s="12"/>
       <c r="AL7" s="12"/>
       <c r="AM7" s="12"/>
+      <c r="AN7" s="12"/>
+      <c r="AO7" s="12"/>
+      <c r="AP7" s="12"/>
+      <c r="AQ7" s="12"/>
+      <c r="AR7" s="12"/>
+      <c r="AS7" s="12"/>
     </row>
-    <row r="8" spans="1:39" ht="16.2" customHeight="1">
+    <row r="8" spans="1:45" ht="16.2" customHeight="1">
       <c r="A8" s="6" t="s">
         <v>68</v>
       </c>
@@ -2939,7 +2949,7 @@
       <c r="Q8" s="20"/>
       <c r="R8" s="20"/>
       <c r="S8" s="20"/>
-      <c r="T8" s="20"/>
+      <c r="T8" s="39"/>
       <c r="U8" s="20"/>
       <c r="V8" s="20"/>
       <c r="W8" s="20"/>
@@ -2959,8 +2969,14 @@
       <c r="AK8" s="20"/>
       <c r="AL8" s="20"/>
       <c r="AM8" s="20"/>
+      <c r="AN8" s="20"/>
+      <c r="AO8" s="20"/>
+      <c r="AP8" s="20"/>
+      <c r="AQ8" s="20"/>
+      <c r="AR8" s="20"/>
+      <c r="AS8" s="20"/>
     </row>
-    <row r="9" spans="1:39" ht="16.2" customHeight="1">
+    <row r="9" spans="1:45" ht="16.2" customHeight="1">
       <c r="A9" s="24" t="s">
         <v>0</v>
       </c>
@@ -2990,10 +3006,8 @@
       <c r="O9" s="21"/>
       <c r="P9" s="21"/>
       <c r="Q9" s="21"/>
-      <c r="R9" s="21"/>
       <c r="S9" s="21"/>
-      <c r="T9" s="21"/>
-      <c r="U9" s="21"/>
+      <c r="T9" s="40"/>
       <c r="V9" s="21"/>
       <c r="W9" s="21"/>
       <c r="X9" s="21"/>
@@ -3012,8 +3026,14 @@
       <c r="AK9" s="21"/>
       <c r="AL9" s="21"/>
       <c r="AM9" s="21"/>
+      <c r="AN9" s="21"/>
+      <c r="AO9" s="21"/>
+      <c r="AP9" s="21"/>
+      <c r="AQ9" s="21"/>
+      <c r="AR9" s="21"/>
+      <c r="AS9" s="21"/>
     </row>
-    <row r="10" spans="1:39" ht="16.2" customHeight="1">
+    <row r="10" spans="1:45" ht="16.2" customHeight="1">
       <c r="A10" s="24" t="s">
         <v>0</v>
       </c>
@@ -3067,8 +3087,14 @@
       <c r="AK10" s="21"/>
       <c r="AL10" s="21"/>
       <c r="AM10" s="21"/>
+      <c r="AN10" s="21"/>
+      <c r="AO10" s="21"/>
+      <c r="AP10" s="21"/>
+      <c r="AQ10" s="21"/>
+      <c r="AR10" s="21"/>
+      <c r="AS10" s="21"/>
     </row>
-    <row r="11" spans="1:39" ht="16.2" customHeight="1">
+    <row r="11" spans="1:45" ht="16.2" customHeight="1">
       <c r="A11" s="24" t="s">
         <v>0</v>
       </c>
@@ -3120,8 +3146,14 @@
       <c r="AK11" s="21"/>
       <c r="AL11" s="21"/>
       <c r="AM11" s="21"/>
+      <c r="AN11" s="21"/>
+      <c r="AO11" s="21"/>
+      <c r="AP11" s="21"/>
+      <c r="AQ11" s="21"/>
+      <c r="AR11" s="21"/>
+      <c r="AS11" s="21"/>
     </row>
-    <row r="12" spans="1:39" ht="16.2" customHeight="1">
+    <row r="12" spans="1:45" ht="16.2" customHeight="1">
       <c r="A12" s="24" t="s">
         <v>0</v>
       </c>
@@ -3175,8 +3207,14 @@
       <c r="AK12" s="21"/>
       <c r="AL12" s="21"/>
       <c r="AM12" s="21"/>
+      <c r="AN12" s="21"/>
+      <c r="AO12" s="21"/>
+      <c r="AP12" s="21"/>
+      <c r="AQ12" s="21"/>
+      <c r="AR12" s="21"/>
+      <c r="AS12" s="21"/>
     </row>
-    <row r="13" spans="1:39" ht="16.2" customHeight="1">
+    <row r="13" spans="1:45" ht="16.2" customHeight="1">
       <c r="A13" s="24" t="s">
         <v>0</v>
       </c>
@@ -3228,8 +3266,14 @@
       <c r="AK13" s="21"/>
       <c r="AL13" s="21"/>
       <c r="AM13" s="21"/>
+      <c r="AN13" s="21"/>
+      <c r="AO13" s="21"/>
+      <c r="AP13" s="21"/>
+      <c r="AQ13" s="21"/>
+      <c r="AR13" s="21"/>
+      <c r="AS13" s="21"/>
     </row>
-    <row r="14" spans="1:39" ht="16.2" customHeight="1">
+    <row r="14" spans="1:45" ht="16.2" customHeight="1">
       <c r="A14" s="24" t="s">
         <v>0</v>
       </c>
@@ -3281,8 +3325,14 @@
       <c r="AK14" s="21"/>
       <c r="AL14" s="21"/>
       <c r="AM14" s="21"/>
+      <c r="AN14" s="21"/>
+      <c r="AO14" s="21"/>
+      <c r="AP14" s="21"/>
+      <c r="AQ14" s="21"/>
+      <c r="AR14" s="21"/>
+      <c r="AS14" s="21"/>
     </row>
-    <row r="15" spans="1:39" ht="16.2" customHeight="1">
+    <row r="15" spans="1:45" ht="16.2" customHeight="1">
       <c r="A15" s="6" t="s">
         <v>68</v>
       </c>
@@ -3336,8 +3386,14 @@
       <c r="AK15" s="20"/>
       <c r="AL15" s="20"/>
       <c r="AM15" s="20"/>
+      <c r="AN15" s="20"/>
+      <c r="AO15" s="20"/>
+      <c r="AP15" s="20"/>
+      <c r="AQ15" s="20"/>
+      <c r="AR15" s="20"/>
+      <c r="AS15" s="20"/>
     </row>
-    <row r="16" spans="1:39" ht="16.2" customHeight="1">
+    <row r="16" spans="1:45" ht="16.2" customHeight="1">
       <c r="A16" s="24" t="s">
         <v>0</v>
       </c>
@@ -3391,8 +3447,14 @@
       <c r="AK16" s="21"/>
       <c r="AL16" s="21"/>
       <c r="AM16" s="21"/>
+      <c r="AN16" s="21"/>
+      <c r="AO16" s="21"/>
+      <c r="AP16" s="21"/>
+      <c r="AQ16" s="21"/>
+      <c r="AR16" s="21"/>
+      <c r="AS16" s="21"/>
     </row>
-    <row r="17" spans="1:39" ht="16.2" customHeight="1">
+    <row r="17" spans="1:45" ht="16.2" customHeight="1">
       <c r="A17" s="6" t="s">
         <v>68</v>
       </c>
@@ -3448,8 +3510,14 @@
       <c r="AK17" s="20"/>
       <c r="AL17" s="20"/>
       <c r="AM17" s="20"/>
+      <c r="AN17" s="20"/>
+      <c r="AO17" s="20"/>
+      <c r="AP17" s="20"/>
+      <c r="AQ17" s="20"/>
+      <c r="AR17" s="20"/>
+      <c r="AS17" s="20"/>
     </row>
-    <row r="18" spans="1:39" ht="16.2" customHeight="1">
+    <row r="18" spans="1:45" ht="16.2" customHeight="1">
       <c r="A18" s="26" t="s">
         <v>104</v>
       </c>
@@ -3503,8 +3571,14 @@
       <c r="AK18" s="21"/>
       <c r="AL18" s="21"/>
       <c r="AM18" s="21"/>
+      <c r="AN18" s="21"/>
+      <c r="AO18" s="21"/>
+      <c r="AP18" s="21"/>
+      <c r="AQ18" s="21"/>
+      <c r="AR18" s="21"/>
+      <c r="AS18" s="21"/>
     </row>
-    <row r="19" spans="1:39" ht="16.2" customHeight="1">
+    <row r="19" spans="1:45" ht="16.2" customHeight="1">
       <c r="A19" s="24" t="s">
         <v>0</v>
       </c>
@@ -3558,8 +3632,14 @@
       <c r="AK19" s="21"/>
       <c r="AL19" s="21"/>
       <c r="AM19" s="21"/>
+      <c r="AN19" s="21"/>
+      <c r="AO19" s="21"/>
+      <c r="AP19" s="21"/>
+      <c r="AQ19" s="21"/>
+      <c r="AR19" s="21"/>
+      <c r="AS19" s="21"/>
     </row>
-    <row r="20" spans="1:39" ht="16.2" customHeight="1">
+    <row r="20" spans="1:45" ht="16.2" customHeight="1">
       <c r="A20" s="24" t="s">
         <v>0</v>
       </c>
@@ -3611,8 +3691,14 @@
       <c r="AK20" s="21"/>
       <c r="AL20" s="21"/>
       <c r="AM20" s="21"/>
+      <c r="AN20" s="21"/>
+      <c r="AO20" s="21"/>
+      <c r="AP20" s="21"/>
+      <c r="AQ20" s="21"/>
+      <c r="AR20" s="21"/>
+      <c r="AS20" s="21"/>
     </row>
-    <row r="21" spans="1:39" ht="16.2" customHeight="1">
+    <row r="21" spans="1:45" ht="16.2" customHeight="1">
       <c r="A21" s="24" t="s">
         <v>0</v>
       </c>
@@ -3664,8 +3750,14 @@
       <c r="AK21" s="21"/>
       <c r="AL21" s="21"/>
       <c r="AM21" s="21"/>
+      <c r="AN21" s="21"/>
+      <c r="AO21" s="21"/>
+      <c r="AP21" s="21"/>
+      <c r="AQ21" s="21"/>
+      <c r="AR21" s="21"/>
+      <c r="AS21" s="21"/>
     </row>
-    <row r="22" spans="1:39" ht="16.2" customHeight="1">
+    <row r="22" spans="1:45" ht="16.2" customHeight="1">
       <c r="A22" s="24" t="s">
         <v>0</v>
       </c>
@@ -3717,8 +3809,14 @@
       <c r="AK22" s="21"/>
       <c r="AL22" s="21"/>
       <c r="AM22" s="21"/>
+      <c r="AN22" s="21"/>
+      <c r="AO22" s="21"/>
+      <c r="AP22" s="21"/>
+      <c r="AQ22" s="21"/>
+      <c r="AR22" s="21"/>
+      <c r="AS22" s="21"/>
     </row>
-    <row r="23" spans="1:39" ht="16.2" customHeight="1">
+    <row r="23" spans="1:45" ht="16.2" customHeight="1">
       <c r="A23" s="24" t="s">
         <v>0</v>
       </c>
@@ -3772,8 +3870,14 @@
       <c r="AK23" s="21"/>
       <c r="AL23" s="21"/>
       <c r="AM23" s="21"/>
+      <c r="AN23" s="21"/>
+      <c r="AO23" s="21"/>
+      <c r="AP23" s="21"/>
+      <c r="AQ23" s="21"/>
+      <c r="AR23" s="21"/>
+      <c r="AS23" s="21"/>
     </row>
-    <row r="24" spans="1:39" ht="24" customHeight="1">
+    <row r="24" spans="1:45" ht="24" customHeight="1">
       <c r="A24" s="11" t="s">
         <v>77</v>
       </c>
@@ -3827,8 +3931,14 @@
       <c r="AK24" s="12"/>
       <c r="AL24" s="12"/>
       <c r="AM24" s="12"/>
+      <c r="AN24" s="12"/>
+      <c r="AO24" s="12"/>
+      <c r="AP24" s="12"/>
+      <c r="AQ24" s="12"/>
+      <c r="AR24" s="12"/>
+      <c r="AS24" s="12"/>
     </row>
-    <row r="25" spans="1:39" ht="16.2" customHeight="1">
+    <row r="25" spans="1:45" ht="16.2" customHeight="1">
       <c r="A25" s="6" t="s">
         <v>68</v>
       </c>
@@ -3882,8 +3992,14 @@
       <c r="AK25" s="20"/>
       <c r="AL25" s="20"/>
       <c r="AM25" s="20"/>
+      <c r="AN25" s="20"/>
+      <c r="AO25" s="20"/>
+      <c r="AP25" s="20"/>
+      <c r="AQ25" s="20"/>
+      <c r="AR25" s="20"/>
+      <c r="AS25" s="20"/>
     </row>
-    <row r="26" spans="1:39" ht="16.2" customHeight="1">
+    <row r="26" spans="1:45" ht="16.2" customHeight="1">
       <c r="A26" s="24" t="s">
         <v>0</v>
       </c>
@@ -3935,8 +4051,14 @@
       <c r="AK26" s="21"/>
       <c r="AL26" s="21"/>
       <c r="AM26" s="21"/>
+      <c r="AN26" s="21"/>
+      <c r="AO26" s="21"/>
+      <c r="AP26" s="21"/>
+      <c r="AQ26" s="21"/>
+      <c r="AR26" s="21"/>
+      <c r="AS26" s="21"/>
     </row>
-    <row r="27" spans="1:39" ht="16.2" customHeight="1">
+    <row r="27" spans="1:45" ht="16.2" customHeight="1">
       <c r="A27" s="24" t="s">
         <v>0</v>
       </c>
@@ -3990,8 +4112,14 @@
       <c r="AK27" s="21"/>
       <c r="AL27" s="21"/>
       <c r="AM27" s="21"/>
+      <c r="AN27" s="21"/>
+      <c r="AO27" s="21"/>
+      <c r="AP27" s="21"/>
+      <c r="AQ27" s="21"/>
+      <c r="AR27" s="21"/>
+      <c r="AS27" s="21"/>
     </row>
-    <row r="28" spans="1:39" ht="16.2" customHeight="1">
+    <row r="28" spans="1:45" ht="16.2" customHeight="1">
       <c r="A28" s="24" t="s">
         <v>0</v>
       </c>
@@ -4043,8 +4171,14 @@
       <c r="AK28" s="21"/>
       <c r="AL28" s="21"/>
       <c r="AM28" s="21"/>
+      <c r="AN28" s="21"/>
+      <c r="AO28" s="21"/>
+      <c r="AP28" s="21"/>
+      <c r="AQ28" s="21"/>
+      <c r="AR28" s="21"/>
+      <c r="AS28" s="21"/>
     </row>
-    <row r="29" spans="1:39" ht="16.2" customHeight="1">
+    <row r="29" spans="1:45" ht="16.2" customHeight="1">
       <c r="A29" s="24" t="s">
         <v>0</v>
       </c>
@@ -4098,8 +4232,14 @@
       <c r="AK29" s="21"/>
       <c r="AL29" s="21"/>
       <c r="AM29" s="21"/>
+      <c r="AN29" s="21"/>
+      <c r="AO29" s="21"/>
+      <c r="AP29" s="21"/>
+      <c r="AQ29" s="21"/>
+      <c r="AR29" s="21"/>
+      <c r="AS29" s="21"/>
     </row>
-    <row r="30" spans="1:39" ht="16.2" customHeight="1">
+    <row r="30" spans="1:45" ht="16.2" customHeight="1">
       <c r="A30" s="24" t="s">
         <v>0</v>
       </c>
@@ -4151,8 +4291,14 @@
       <c r="AK30" s="21"/>
       <c r="AL30" s="21"/>
       <c r="AM30" s="21"/>
+      <c r="AN30" s="21"/>
+      <c r="AO30" s="21"/>
+      <c r="AP30" s="21"/>
+      <c r="AQ30" s="21"/>
+      <c r="AR30" s="21"/>
+      <c r="AS30" s="21"/>
     </row>
-    <row r="31" spans="1:39" ht="16.2" customHeight="1">
+    <row r="31" spans="1:45" ht="16.2" customHeight="1">
       <c r="A31" s="24" t="s">
         <v>0</v>
       </c>
@@ -4204,8 +4350,14 @@
       <c r="AK31" s="21"/>
       <c r="AL31" s="21"/>
       <c r="AM31" s="21"/>
+      <c r="AN31" s="21"/>
+      <c r="AO31" s="21"/>
+      <c r="AP31" s="21"/>
+      <c r="AQ31" s="21"/>
+      <c r="AR31" s="21"/>
+      <c r="AS31" s="21"/>
     </row>
-    <row r="32" spans="1:39" ht="16.2" customHeight="1">
+    <row r="32" spans="1:45" ht="16.2" customHeight="1">
       <c r="A32" s="6" t="s">
         <v>68</v>
       </c>
@@ -4259,8 +4411,14 @@
       <c r="AK32" s="20"/>
       <c r="AL32" s="20"/>
       <c r="AM32" s="20"/>
+      <c r="AN32" s="20"/>
+      <c r="AO32" s="20"/>
+      <c r="AP32" s="20"/>
+      <c r="AQ32" s="20"/>
+      <c r="AR32" s="20"/>
+      <c r="AS32" s="20"/>
     </row>
-    <row r="33" spans="1:39" ht="16.2" customHeight="1">
+    <row r="33" spans="1:45" ht="16.2" customHeight="1">
       <c r="A33" s="24" t="s">
         <v>0</v>
       </c>
@@ -4314,8 +4472,14 @@
       <c r="AK33" s="21"/>
       <c r="AL33" s="21"/>
       <c r="AM33" s="21"/>
+      <c r="AN33" s="21"/>
+      <c r="AO33" s="21"/>
+      <c r="AP33" s="21"/>
+      <c r="AQ33" s="21"/>
+      <c r="AR33" s="21"/>
+      <c r="AS33" s="21"/>
     </row>
-    <row r="34" spans="1:39" ht="16.2" customHeight="1">
+    <row r="34" spans="1:45" ht="16.2" customHeight="1">
       <c r="A34" s="24" t="s">
         <v>0</v>
       </c>
@@ -4369,8 +4533,14 @@
       <c r="AK34" s="21"/>
       <c r="AL34" s="21"/>
       <c r="AM34" s="21"/>
+      <c r="AN34" s="21"/>
+      <c r="AO34" s="21"/>
+      <c r="AP34" s="21"/>
+      <c r="AQ34" s="21"/>
+      <c r="AR34" s="21"/>
+      <c r="AS34" s="21"/>
     </row>
-    <row r="35" spans="1:39" ht="16.2" customHeight="1">
+    <row r="35" spans="1:45" ht="16.2" customHeight="1">
       <c r="A35" s="6" t="s">
         <v>68</v>
       </c>
@@ -4426,8 +4596,14 @@
       <c r="AK35" s="20"/>
       <c r="AL35" s="20"/>
       <c r="AM35" s="20"/>
+      <c r="AN35" s="20"/>
+      <c r="AO35" s="20"/>
+      <c r="AP35" s="20"/>
+      <c r="AQ35" s="20"/>
+      <c r="AR35" s="20"/>
+      <c r="AS35" s="20"/>
     </row>
-    <row r="36" spans="1:39" ht="16.2" customHeight="1">
+    <row r="36" spans="1:45" ht="16.2" customHeight="1">
       <c r="A36" s="26" t="s">
         <v>104</v>
       </c>
@@ -4481,8 +4657,14 @@
       <c r="AK36" s="21"/>
       <c r="AL36" s="21"/>
       <c r="AM36" s="21"/>
+      <c r="AN36" s="21"/>
+      <c r="AO36" s="21"/>
+      <c r="AP36" s="21"/>
+      <c r="AQ36" s="21"/>
+      <c r="AR36" s="21"/>
+      <c r="AS36" s="21"/>
     </row>
-    <row r="37" spans="1:39" ht="16.2" customHeight="1">
+    <row r="37" spans="1:45" ht="16.2" customHeight="1">
       <c r="A37" s="24" t="s">
         <v>0</v>
       </c>
@@ -4536,8 +4718,14 @@
       <c r="AK37" s="21"/>
       <c r="AL37" s="21"/>
       <c r="AM37" s="21"/>
+      <c r="AN37" s="21"/>
+      <c r="AO37" s="21"/>
+      <c r="AP37" s="21"/>
+      <c r="AQ37" s="21"/>
+      <c r="AR37" s="21"/>
+      <c r="AS37" s="21"/>
     </row>
-    <row r="38" spans="1:39" ht="16.2" customHeight="1">
+    <row r="38" spans="1:45" ht="16.2" customHeight="1">
       <c r="A38" s="24" t="s">
         <v>0</v>
       </c>
@@ -4591,8 +4779,14 @@
       <c r="AK38" s="21"/>
       <c r="AL38" s="21"/>
       <c r="AM38" s="21"/>
+      <c r="AN38" s="21"/>
+      <c r="AO38" s="21"/>
+      <c r="AP38" s="21"/>
+      <c r="AQ38" s="21"/>
+      <c r="AR38" s="21"/>
+      <c r="AS38" s="21"/>
     </row>
-    <row r="39" spans="1:39" ht="16.2" customHeight="1">
+    <row r="39" spans="1:45" ht="16.2" customHeight="1">
       <c r="A39" s="24" t="s">
         <v>0</v>
       </c>
@@ -4644,8 +4838,14 @@
       <c r="AK39" s="21"/>
       <c r="AL39" s="21"/>
       <c r="AM39" s="21"/>
+      <c r="AN39" s="21"/>
+      <c r="AO39" s="21"/>
+      <c r="AP39" s="21"/>
+      <c r="AQ39" s="21"/>
+      <c r="AR39" s="21"/>
+      <c r="AS39" s="21"/>
     </row>
-    <row r="40" spans="1:39" ht="16.2" customHeight="1">
+    <row r="40" spans="1:45" ht="16.2" customHeight="1">
       <c r="A40" s="24" t="s">
         <v>0</v>
       </c>
@@ -4697,8 +4897,14 @@
       <c r="AK40" s="21"/>
       <c r="AL40" s="21"/>
       <c r="AM40" s="21"/>
+      <c r="AN40" s="21"/>
+      <c r="AO40" s="21"/>
+      <c r="AP40" s="21"/>
+      <c r="AQ40" s="21"/>
+      <c r="AR40" s="21"/>
+      <c r="AS40" s="21"/>
     </row>
-    <row r="41" spans="1:39" ht="16.2" customHeight="1">
+    <row r="41" spans="1:45" ht="16.2" customHeight="1">
       <c r="A41" s="24" t="s">
         <v>0</v>
       </c>
@@ -4750,8 +4956,14 @@
       <c r="AK41" s="21"/>
       <c r="AL41" s="21"/>
       <c r="AM41" s="21"/>
+      <c r="AN41" s="21"/>
+      <c r="AO41" s="21"/>
+      <c r="AP41" s="21"/>
+      <c r="AQ41" s="21"/>
+      <c r="AR41" s="21"/>
+      <c r="AS41" s="21"/>
     </row>
-    <row r="42" spans="1:39" ht="16.2" customHeight="1">
+    <row r="42" spans="1:45" ht="16.2" customHeight="1">
       <c r="A42" s="24" t="s">
         <v>0</v>
       </c>
@@ -4803,8 +5015,14 @@
       <c r="AK42" s="21"/>
       <c r="AL42" s="21"/>
       <c r="AM42" s="21"/>
+      <c r="AN42" s="21"/>
+      <c r="AO42" s="21"/>
+      <c r="AP42" s="21"/>
+      <c r="AQ42" s="21"/>
+      <c r="AR42" s="21"/>
+      <c r="AS42" s="21"/>
     </row>
-    <row r="43" spans="1:39" ht="16.2" customHeight="1">
+    <row r="43" spans="1:45" ht="16.2" customHeight="1">
       <c r="A43" s="27" t="s">
         <v>0</v>
       </c>
@@ -4856,8 +5074,14 @@
       <c r="AK43" s="22"/>
       <c r="AL43" s="22"/>
       <c r="AM43" s="22"/>
+      <c r="AN43" s="22"/>
+      <c r="AO43" s="22"/>
+      <c r="AP43" s="22"/>
+      <c r="AQ43" s="22"/>
+      <c r="AR43" s="22"/>
+      <c r="AS43" s="22"/>
     </row>
-    <row r="44" spans="1:39" ht="16.2" customHeight="1">
+    <row r="44" spans="1:45" ht="16.2" customHeight="1">
       <c r="A44" s="7"/>
       <c r="B44" s="7"/>
       <c r="C44" s="7"/>
@@ -4866,7 +5090,7 @@
       <c r="I44" s="8"/>
       <c r="J44" s="8"/>
     </row>
-    <row r="45" spans="1:39" ht="22.8" customHeight="1">
+    <row r="45" spans="1:45" ht="22.95" customHeight="1">
       <c r="A45" s="9" t="s">
         <v>73</v>
       </c>
@@ -4922,8 +5146,14 @@
       <c r="AK45" s="10"/>
       <c r="AL45" s="10"/>
       <c r="AM45" s="10"/>
+      <c r="AN45" s="10"/>
+      <c r="AO45" s="10"/>
+      <c r="AP45" s="10"/>
+      <c r="AQ45" s="10"/>
+      <c r="AR45" s="10"/>
+      <c r="AS45" s="10"/>
     </row>
-    <row r="46" spans="1:39" ht="16.2" customHeight="1">
+    <row r="46" spans="1:45" ht="16.2" customHeight="1">
       <c r="A46" s="7"/>
       <c r="B46" s="7"/>
       <c r="C46" s="7"/>
@@ -4932,7 +5162,7 @@
       <c r="I46" s="8"/>
       <c r="J46" s="8"/>
     </row>
-    <row r="47" spans="1:39" ht="22.8" customHeight="1">
+    <row r="47" spans="1:45" ht="22.95" customHeight="1">
       <c r="A47" s="9" t="s">
         <v>73</v>
       </c>
@@ -4988,18 +5218,27 @@
       <c r="AK47" s="10"/>
       <c r="AL47" s="10"/>
       <c r="AM47" s="10"/>
+      <c r="AN47" s="10"/>
+      <c r="AO47" s="10"/>
+      <c r="AP47" s="10"/>
+      <c r="AQ47" s="10"/>
+      <c r="AR47" s="10"/>
+      <c r="AS47" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="F4:H32 F34:H47">
-    <cfRule type="expression" dxfId="4" priority="4">
+    <cfRule type="expression" dxfId="45" priority="5">
       <formula>LEN(D4)&gt;150</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F33:H33">
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="44" priority="3">
       <formula>LEN(D33)&gt;150</formula>
     </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="duplicateValues" dxfId="43" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>